<commit_message>
tests for output and expoutput
</commit_message>
<xml_diff>
--- a/tests/TestFiles/expoutput/mainconfig.xlsx
+++ b/tests/TestFiles/expoutput/mainconfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\tests\TestFiles\expoutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D479D8-D77D-4711-AAEB-D6B77BF755A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85124D6-4701-409E-AAE2-100533CCEF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="1620" windowWidth="18000" windowHeight="9360" firstSheet="1" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="1635" yWindow="1620" windowWidth="18000" windowHeight="9360" firstSheet="1" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="96">
   <si>
     <t>Default Benchmarks</t>
   </si>
@@ -265,13 +265,76 @@
   </si>
   <si>
     <t>SphereSDDR</t>
+  </si>
+  <si>
+    <t>Tiara BC scintillator detector</t>
+  </si>
+  <si>
+    <t>Tiara-BC</t>
+  </si>
+  <si>
+    <t>Tiara Bonner Sphere detector</t>
+  </si>
+  <si>
+    <t>Tiara-BS</t>
+  </si>
+  <si>
+    <t>Tiara Fission Chambers detector</t>
+  </si>
+  <si>
+    <t>Tiara-FC</t>
+  </si>
+  <si>
+    <t>FNS Time-of-Flight Experiment</t>
+  </si>
+  <si>
+    <t>FNS-TOF</t>
+  </si>
+  <si>
+    <t>FNG Bulk Blanket and Shielding Experiment</t>
+  </si>
+  <si>
+    <t>FNG-BKT</t>
+  </si>
+  <si>
+    <t>FNG Tungsten</t>
+  </si>
+  <si>
+    <t>FNG-W</t>
+  </si>
+  <si>
+    <t>ASPIS Iron-88 benchmark</t>
+  </si>
+  <si>
+    <t>ASPIS-Fe88</t>
+  </si>
+  <si>
+    <t>Iron Slab Experiment (TUD)</t>
+  </si>
+  <si>
+    <t>TUD-Fe</t>
+  </si>
+  <si>
+    <t>TUD Spectra Measurements (FNG Bulk Shield)</t>
+  </si>
+  <si>
+    <t>TUD-FNG</t>
+  </si>
+  <si>
+    <t>FNG/TUD Tungsten Experiment</t>
+  </si>
+  <si>
+    <t>TUD-W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000000"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +387,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -435,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -461,9 +530,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,6 +573,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -836,10 +911,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -869,7 +944,7 @@
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>49</v>
       </c>
     </row>
@@ -890,7 +965,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -898,38 +973,38 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="18"/>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="18"/>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>61</v>
       </c>
     </row>
@@ -954,307 +1029,307 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="13" customWidth="1"/>
-    <col min="4" max="7" width="9.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="10" style="13" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="13" customWidth="1"/>
-    <col min="10" max="10" width="9" style="13" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="13"/>
+    <col min="1" max="1" width="24.85546875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="12" customWidth="1"/>
+    <col min="4" max="7" width="9.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="10" style="12" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="12" customWidth="1"/>
+    <col min="10" max="10" width="9" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-    </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="1:10" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="17">
+      <c r="C4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="16">
         <v>10000</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="16" t="s">
+      <c r="E5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="16">
         <v>10000</v>
       </c>
-      <c r="J5" s="16"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="17">
+      <c r="C6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="16">
         <v>1000</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="17">
+      <c r="C7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="16">
         <v>1000</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="17">
+      <c r="D8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="16">
         <v>1000</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="17">
+      <c r="C9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="16">
         <v>1000000</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="17">
+      <c r="C10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="16">
         <v>100000000</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1269,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,172 +1362,418 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10" t="s">
+      <c r="E4" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="11">
-        <v>1000000</v>
+      <c r="I4" s="27">
+        <v>100</v>
       </c>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="11">
-        <v>10000</v>
+      <c r="C5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="27">
+        <v>500000000</v>
       </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="A6" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="27">
+        <v>100</v>
+      </c>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="A7" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="27">
+        <v>100</v>
+      </c>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="A8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="27">
+        <v>100</v>
+      </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="A9" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="27">
+        <v>100</v>
+      </c>
       <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="27">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
update expoutput test coverage
</commit_message>
<xml_diff>
--- a/tests/TestFiles/expoutput/mainconfig.xlsx
+++ b/tests/TestFiles/expoutput/mainconfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\laghida\Documents\GitHub\JADE\tests\TestFiles\expoutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\tests\TestFiles\expoutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C159C-B886-433B-B1DD-33262C337623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836EF406-F81A-482D-81B2-13BBA57C0599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -903,23 +903,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1A2DE-3EB8-4AD4-9CF1-023800AFF144}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.453125" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
     <col min="2" max="2" width="106" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="24"/>
     </row>
-    <row r="2" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -927,7 +927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -935,7 +935,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
@@ -943,7 +943,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -951,7 +951,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
@@ -959,7 +959,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -967,7 +967,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>54</v>
       </c>
@@ -975,19 +975,19 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="18"/>
     </row>
-    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="18"/>
     </row>
-    <row r="11" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>58</v>
       </c>
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>59</v>
       </c>
@@ -1003,13 +1003,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>96</v>
       </c>
       <c r="B13" s="18"/>
     </row>
-    <row r="14" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>60</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
@@ -1042,19 +1042,19 @@
       <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" style="12" customWidth="1"/>
-    <col min="4" max="7" width="9.453125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="12" customWidth="1"/>
+    <col min="4" max="7" width="9.42578125" style="12" customWidth="1"/>
     <col min="8" max="8" width="10" style="12" customWidth="1"/>
-    <col min="9" max="9" width="8.81640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="12" customWidth="1"/>
     <col min="10" max="10" width="9" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="8.81640625" style="12"/>
+    <col min="11" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>19</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
     </row>
-    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
     </row>
-    <row r="3" spans="1:10" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="J5" s="15"/>
     </row>
-    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="J6" s="15"/>
     </row>
-    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>31</v>
       </c>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="J7" s="15"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>32</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="J9" s="15"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -1355,22 +1355,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="7" width="9.453125" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" customWidth="1"/>
-    <col min="10" max="10" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
@@ -1384,7 +1384,7 @@
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
     </row>
-    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>27</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>39</v>
       </c>
@@ -1479,8 +1479,8 @@
       <c r="F5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>24</v>
+      <c r="G5" s="20" t="s">
+        <v>23</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>24</v>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>76</v>
       </c>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>78</v>
       </c>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>80</v>
       </c>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>82</v>
       </c>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>84</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>86</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>88</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>90</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>92</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>94</v>
       </c>
@@ -1802,17 +1802,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1"/>
-    <col min="2" max="2" width="18.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.453125" customWidth="1"/>
-    <col min="5" max="5" width="31.81640625" customWidth="1"/>
-    <col min="6" max="6" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>